<commit_message>
Interface and back-end for start screen and characters
</commit_message>
<xml_diff>
--- a/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SOhlrich_timelog.xlsx
+++ b/SD4_kkleber_sohlrich_rsanders_sspangler/SD4_kkleber_sohlrich_rsanders_sspangler/Documents/SD4_SOhlrich_timelog.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="294">
   <si>
     <t>Date:</t>
   </si>
@@ -1408,6 +1408,21 @@
   </si>
   <si>
     <t>"Are these designs thorough enough for the project?"</t>
+  </si>
+  <si>
+    <t>Components will be coded/iterated through, if any components are not thoroughly designed then they will be brought back to the design phase.</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>Main menu too</t>
+  </si>
+  <si>
+    <t>Main menu</t>
+  </si>
+  <si>
+    <t>Character menu</t>
   </si>
 </sst>
 </file>
@@ -1869,7 +1884,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2108,6 +2123,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
@@ -3056,8 +3074,8 @@
   <dimension ref="A1:J121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="12" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3100,7 +3118,7 @@
       <c r="C3" s="57"/>
       <c r="H3" s="70">
         <f>SUM(G13:G121)</f>
-        <v>6.6666666666666707E-2</v>
+        <v>0.19375000000000012</v>
       </c>
       <c r="I3" t="s">
         <v>171</v>
@@ -3113,7 +3131,7 @@
       <c r="C4" s="27"/>
       <c r="H4" s="71">
         <f>(INT(H3*24))+MINUTE(H3)/60</f>
-        <v>1.6</v>
+        <v>4.6500000000000004</v>
       </c>
       <c r="I4" t="s">
         <v>171</v>
@@ -3321,34 +3339,127 @@
         <v>288</v>
       </c>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0.72291666666666676</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0.73055555555555562</v>
+      </c>
+      <c r="F18" s="91">
+        <v>3</v>
+      </c>
       <c r="G18" s="8">
         <f t="shared" ref="G18:G20" si="1">(E18-D18)-(F18/1440)</f>
-        <v>0</v>
+        <v>5.5555555555555289E-3</v>
+      </c>
+      <c r="H18" t="s">
+        <v>276</v>
+      </c>
+      <c r="I18" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="101" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D19" s="5">
+        <v>0.84861111111111109</v>
+      </c>
+      <c r="E19" s="5">
+        <v>0.86805555555555547</v>
+      </c>
       <c r="G19" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.9444444444444375E-2</v>
+      </c>
+      <c r="H19" t="s">
+        <v>290</v>
+      </c>
+      <c r="I19" t="s">
+        <v>52</v>
+      </c>
+      <c r="J19" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D20" s="5">
+        <v>0.58819444444444446</v>
+      </c>
+      <c r="E20" s="5">
+        <v>0.67152777777777783</v>
+      </c>
+      <c r="F20" s="91">
+        <v>45</v>
+      </c>
       <c r="G20" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="H20" t="s">
+        <v>290</v>
+      </c>
+      <c r="I20" t="s">
+        <v>52</v>
+      </c>
+      <c r="J20" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0.7597222222222223</v>
+      </c>
+      <c r="F21" s="91">
+        <v>10</v>
+      </c>
       <c r="G21" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.6805555555555619E-2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>290</v>
+      </c>
+      <c r="I21" t="s">
+        <v>52</v>
+      </c>
+      <c r="J21" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>42120</v>
+      </c>
+      <c r="D22" s="5">
+        <v>0.87708333333333333</v>
+      </c>
+      <c r="E22" s="5">
+        <v>0.89027777777777783</v>
+      </c>
       <c r="G22" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3194444444444509E-2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="23" spans="3:10" x14ac:dyDescent="0.25">
@@ -5799,42 +5910,42 @@
       <c r="B5" s="3"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" s="101" t="s">
+      <c r="B6" s="102" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="101"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-      <c r="I6" s="101"/>
-      <c r="J6" s="101"/>
-      <c r="K6" s="101"/>
-      <c r="L6" s="101"/>
-      <c r="M6" s="101"/>
-      <c r="N6" s="101"/>
-      <c r="O6" s="101"/>
-      <c r="P6" s="101"/>
+      <c r="C6" s="102"/>
+      <c r="D6" s="102"/>
+      <c r="E6" s="102"/>
+      <c r="F6" s="102"/>
+      <c r="G6" s="102"/>
+      <c r="H6" s="102"/>
+      <c r="I6" s="102"/>
+      <c r="J6" s="102"/>
+      <c r="K6" s="102"/>
+      <c r="L6" s="102"/>
+      <c r="M6" s="102"/>
+      <c r="N6" s="102"/>
+      <c r="O6" s="102"/>
+      <c r="P6" s="102"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B7" s="101" t="s">
+      <c r="B7" s="102" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="101"/>
-      <c r="D7" s="101"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-      <c r="I7" s="101"/>
-      <c r="J7" s="101"/>
-      <c r="K7" s="101"/>
-      <c r="L7" s="101"/>
-      <c r="M7" s="101"/>
-      <c r="N7" s="101"/>
-      <c r="O7" s="101"/>
-      <c r="P7" s="101"/>
+      <c r="C7" s="102"/>
+      <c r="D7" s="102"/>
+      <c r="E7" s="102"/>
+      <c r="F7" s="102"/>
+      <c r="G7" s="102"/>
+      <c r="H7" s="102"/>
+      <c r="I7" s="102"/>
+      <c r="J7" s="102"/>
+      <c r="K7" s="102"/>
+      <c r="L7" s="102"/>
+      <c r="M7" s="102"/>
+      <c r="N7" s="102"/>
+      <c r="O7" s="102"/>
+      <c r="P7" s="102"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
@@ -5845,55 +5956,55 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B10" s="101" t="s">
+      <c r="B10" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="101"/>
-      <c r="D10" s="101"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-      <c r="I10" s="101"/>
-      <c r="J10" s="101"/>
-      <c r="K10" s="101"/>
-      <c r="L10" s="101"/>
-      <c r="M10" s="101"/>
-      <c r="N10" s="101"/>
-      <c r="O10" s="101"/>
-      <c r="P10" s="101"/>
+      <c r="C10" s="102"/>
+      <c r="D10" s="102"/>
+      <c r="E10" s="102"/>
+      <c r="F10" s="102"/>
+      <c r="G10" s="102"/>
+      <c r="H10" s="102"/>
+      <c r="I10" s="102"/>
+      <c r="J10" s="102"/>
+      <c r="K10" s="102"/>
+      <c r="L10" s="102"/>
+      <c r="M10" s="102"/>
+      <c r="N10" s="102"/>
+      <c r="O10" s="102"/>
+      <c r="P10" s="102"/>
     </row>
     <row r="11" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="105" t="s">
+      <c r="C11" s="106" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="101"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-      <c r="I11" s="101"/>
-      <c r="J11" s="101"/>
-      <c r="K11" s="101"/>
+      <c r="D11" s="102"/>
+      <c r="E11" s="102"/>
+      <c r="F11" s="102"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="102"/>
+      <c r="I11" s="102"/>
+      <c r="J11" s="102"/>
+      <c r="K11" s="102"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="101"/>
-      <c r="D12" s="101"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-      <c r="I12" s="101"/>
-      <c r="J12" s="101"/>
-      <c r="K12" s="101"/>
-      <c r="L12" s="101"/>
-      <c r="M12" s="101"/>
-      <c r="N12" s="101"/>
-      <c r="O12" s="101"/>
-      <c r="P12" s="101"/>
+      <c r="C12" s="102"/>
+      <c r="D12" s="102"/>
+      <c r="E12" s="102"/>
+      <c r="F12" s="102"/>
+      <c r="G12" s="102"/>
+      <c r="H12" s="102"/>
+      <c r="I12" s="102"/>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" s="102"/>
+      <c r="O12" s="102"/>
+      <c r="P12" s="102"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C13" s="11" t="s">
@@ -5901,36 +6012,36 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="101"/>
-      <c r="K14" s="101"/>
-      <c r="L14" s="101"/>
-      <c r="M14" s="101"/>
-      <c r="N14" s="101"/>
-      <c r="O14" s="101"/>
+      <c r="C14" s="102"/>
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C15" s="102" t="s">
+      <c r="C15" s="103" t="s">
         <v>29</v>
       </c>
-      <c r="D15" s="101"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="101"/>
-      <c r="K15" s="101"/>
-      <c r="L15" s="101"/>
+      <c r="D15" s="102"/>
+      <c r="E15" s="102"/>
+      <c r="F15" s="102"/>
+      <c r="G15" s="102"/>
+      <c r="H15" s="102"/>
+      <c r="I15" s="102"/>
+      <c r="J15" s="102"/>
+      <c r="K15" s="102"/>
+      <c r="L15" s="102"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
@@ -5961,187 +6072,187 @@
     </row>
     <row r="18" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B18" s="14"/>
-      <c r="C18" s="104" t="s">
+      <c r="C18" s="105" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="101"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="101"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="101"/>
-      <c r="J18" s="101"/>
-      <c r="K18" s="101"/>
-      <c r="L18" s="101"/>
-      <c r="M18" s="101"/>
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="102"/>
+      <c r="H18" s="102"/>
+      <c r="I18" s="102"/>
+      <c r="J18" s="102"/>
+      <c r="K18" s="102"/>
+      <c r="L18" s="102"/>
+      <c r="M18" s="102"/>
       <c r="N18" s="14"/>
       <c r="O18" s="14"/>
     </row>
     <row r="19" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
-      <c r="D19" s="103" t="s">
+      <c r="D19" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="101"/>
-      <c r="F19" s="101"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="101"/>
-      <c r="J19" s="101"/>
-      <c r="K19" s="101"/>
-      <c r="L19" s="101"/>
-      <c r="M19" s="101"/>
+      <c r="E19" s="102"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="102"/>
+      <c r="H19" s="102"/>
+      <c r="I19" s="102"/>
+      <c r="J19" s="102"/>
+      <c r="K19" s="102"/>
+      <c r="L19" s="102"/>
+      <c r="M19" s="102"/>
       <c r="N19" s="14"/>
       <c r="O19" s="14"/>
     </row>
     <row r="20" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B20" s="14"/>
-      <c r="C20" s="103" t="s">
+      <c r="C20" s="104" t="s">
         <v>34</v>
       </c>
-      <c r="D20" s="101"/>
-      <c r="E20" s="101"/>
-      <c r="F20" s="101"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-      <c r="I20" s="101"/>
-      <c r="J20" s="101"/>
-      <c r="K20" s="101"/>
-      <c r="L20" s="101"/>
-      <c r="M20" s="101"/>
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102"/>
+      <c r="H20" s="102"/>
+      <c r="I20" s="102"/>
+      <c r="J20" s="102"/>
+      <c r="K20" s="102"/>
+      <c r="L20" s="102"/>
+      <c r="M20" s="102"/>
       <c r="N20" s="14"/>
       <c r="O20" s="14"/>
     </row>
     <row r="21" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B21" s="14"/>
       <c r="C21" s="15"/>
-      <c r="D21" s="101" t="s">
+      <c r="D21" s="102" t="s">
         <v>35</v>
       </c>
-      <c r="E21" s="101"/>
-      <c r="F21" s="101"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101"/>
-      <c r="I21" s="101"/>
-      <c r="J21" s="101"/>
-      <c r="K21" s="101"/>
-      <c r="L21" s="101"/>
-      <c r="M21" s="101"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="102"/>
+      <c r="G21" s="102"/>
+      <c r="H21" s="102"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="102"/>
+      <c r="K21" s="102"/>
+      <c r="L21" s="102"/>
+      <c r="M21" s="102"/>
       <c r="N21" s="14"/>
       <c r="O21" s="14"/>
     </row>
     <row r="22" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B22" s="14"/>
       <c r="C22" s="15"/>
-      <c r="D22" s="101" t="s">
+      <c r="D22" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="E22" s="101"/>
-      <c r="F22" s="101"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
-      <c r="I22" s="101"/>
-      <c r="J22" s="101"/>
-      <c r="K22" s="101"/>
-      <c r="L22" s="101"/>
-      <c r="M22" s="101"/>
-      <c r="N22" s="101"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102"/>
+      <c r="H22" s="102"/>
+      <c r="I22" s="102"/>
+      <c r="J22" s="102"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="102"/>
+      <c r="M22" s="102"/>
+      <c r="N22" s="102"/>
       <c r="O22" s="14"/>
     </row>
     <row r="23" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B23" s="14"/>
       <c r="C23" s="15"/>
-      <c r="D23" s="101" t="s">
+      <c r="D23" s="102" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="101"/>
-      <c r="L23" s="101"/>
-      <c r="M23" s="101"/>
-      <c r="N23" s="101"/>
-      <c r="O23" s="101"/>
-      <c r="P23" s="101"/>
-      <c r="Q23" s="101"/>
+      <c r="E23" s="102"/>
+      <c r="F23" s="102"/>
+      <c r="G23" s="102"/>
+      <c r="H23" s="102"/>
+      <c r="I23" s="102"/>
+      <c r="J23" s="102"/>
+      <c r="K23" s="102"/>
+      <c r="L23" s="102"/>
+      <c r="M23" s="102"/>
+      <c r="N23" s="102"/>
+      <c r="O23" s="102"/>
+      <c r="P23" s="102"/>
+      <c r="Q23" s="102"/>
     </row>
     <row r="24" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B24" s="14"/>
       <c r="C24" s="15"/>
-      <c r="D24" s="101" t="s">
+      <c r="D24" s="102" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="101"/>
-      <c r="F24" s="101"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-      <c r="I24" s="101"/>
-      <c r="J24" s="101"/>
-      <c r="K24" s="101"/>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="101"/>
-      <c r="P24" s="101"/>
-      <c r="Q24" s="101"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102"/>
+      <c r="H24" s="102"/>
+      <c r="I24" s="102"/>
+      <c r="J24" s="102"/>
+      <c r="K24" s="102"/>
+      <c r="L24" s="102"/>
+      <c r="M24" s="102"/>
+      <c r="N24" s="102"/>
+      <c r="O24" s="102"/>
+      <c r="P24" s="102"/>
+      <c r="Q24" s="102"/>
     </row>
     <row r="25" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B25" s="14"/>
       <c r="C25" s="15"/>
-      <c r="D25" s="101" t="s">
+      <c r="D25" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="101"/>
-      <c r="F25" s="101"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="101"/>
-      <c r="I25" s="101"/>
-      <c r="J25" s="101"/>
-      <c r="K25" s="101"/>
-      <c r="L25" s="101"/>
-      <c r="M25" s="101"/>
-      <c r="N25" s="101"/>
-      <c r="O25" s="101"/>
-      <c r="P25" s="101"/>
-      <c r="Q25" s="101"/>
+      <c r="E25" s="102"/>
+      <c r="F25" s="102"/>
+      <c r="G25" s="102"/>
+      <c r="H25" s="102"/>
+      <c r="I25" s="102"/>
+      <c r="J25" s="102"/>
+      <c r="K25" s="102"/>
+      <c r="L25" s="102"/>
+      <c r="M25" s="102"/>
+      <c r="N25" s="102"/>
+      <c r="O25" s="102"/>
+      <c r="P25" s="102"/>
+      <c r="Q25" s="102"/>
     </row>
     <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="14"/>
-      <c r="C26" s="103" t="s">
+      <c r="C26" s="104" t="s">
         <v>41</v>
       </c>
-      <c r="D26" s="101"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="101"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-      <c r="I26" s="101"/>
-      <c r="J26" s="101"/>
-      <c r="K26" s="101"/>
-      <c r="L26" s="101"/>
-      <c r="M26" s="101"/>
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="102"/>
+      <c r="H26" s="102"/>
+      <c r="I26" s="102"/>
+      <c r="J26" s="102"/>
+      <c r="K26" s="102"/>
+      <c r="L26" s="102"/>
+      <c r="M26" s="102"/>
       <c r="N26" s="14"/>
       <c r="O26" s="14"/>
     </row>
     <row r="27" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B27" s="14"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="101" t="s">
+      <c r="D27" s="102" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="101"/>
-      <c r="F27" s="101"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-      <c r="I27" s="101"/>
-      <c r="J27" s="101"/>
-      <c r="K27" s="101"/>
-      <c r="L27" s="101"/>
-      <c r="M27" s="101"/>
+      <c r="E27" s="102"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="102"/>
+      <c r="H27" s="102"/>
+      <c r="I27" s="102"/>
+      <c r="J27" s="102"/>
+      <c r="K27" s="102"/>
+      <c r="L27" s="102"/>
+      <c r="M27" s="102"/>
       <c r="N27" s="14"/>
       <c r="O27" s="14"/>
     </row>
@@ -6172,84 +6283,84 @@
       </c>
     </row>
     <row r="32" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C32" s="102" t="s">
+      <c r="C32" s="103" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="101"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="101"/>
-      <c r="G32" s="101"/>
-      <c r="H32" s="101"/>
-      <c r="I32" s="101"/>
-      <c r="J32" s="101"/>
-      <c r="K32" s="101"/>
-      <c r="L32" s="101"/>
-      <c r="M32" s="101"/>
-      <c r="N32" s="101"/>
+      <c r="D32" s="102"/>
+      <c r="E32" s="102"/>
+      <c r="F32" s="102"/>
+      <c r="G32" s="102"/>
+      <c r="H32" s="102"/>
+      <c r="I32" s="102"/>
+      <c r="J32" s="102"/>
+      <c r="K32" s="102"/>
+      <c r="L32" s="102"/>
+      <c r="M32" s="102"/>
+      <c r="N32" s="102"/>
     </row>
     <row r="34" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="101" t="s">
+      <c r="C34" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="101"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="101"/>
-      <c r="G34" s="101"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="101"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="102"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="102"/>
+      <c r="J34" s="102"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="102"/>
+      <c r="M34" s="102"/>
+      <c r="N34" s="102"/>
     </row>
     <row r="35" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="102" t="s">
+      <c r="C35" s="103" t="s">
         <v>23</v>
       </c>
-      <c r="D35" s="101"/>
-      <c r="E35" s="101"/>
-      <c r="F35" s="101"/>
-      <c r="G35" s="101"/>
-      <c r="H35" s="101"/>
-      <c r="I35" s="101"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="101"/>
-      <c r="L35" s="101"/>
-      <c r="M35" s="101"/>
-      <c r="N35" s="101"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="102"/>
+      <c r="I35" s="102"/>
+      <c r="J35" s="102"/>
+      <c r="K35" s="102"/>
+      <c r="L35" s="102"/>
+      <c r="M35" s="102"/>
+      <c r="N35" s="102"/>
     </row>
     <row r="37" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="101" t="s">
+      <c r="C37" s="102" t="s">
         <v>24</v>
       </c>
-      <c r="D37" s="101"/>
-      <c r="E37" s="101"/>
-      <c r="F37" s="101"/>
-      <c r="G37" s="101"/>
-      <c r="H37" s="101"/>
-      <c r="I37" s="101"/>
-      <c r="J37" s="101"/>
-      <c r="K37" s="101"/>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
-      <c r="N37" s="101"/>
+      <c r="D37" s="102"/>
+      <c r="E37" s="102"/>
+      <c r="F37" s="102"/>
+      <c r="G37" s="102"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="102"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="102"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="102"/>
     </row>
     <row r="38" spans="3:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="102" t="s">
+      <c r="C38" s="103" t="s">
         <v>25</v>
       </c>
-      <c r="D38" s="101"/>
-      <c r="E38" s="101"/>
-      <c r="F38" s="101"/>
-      <c r="G38" s="101"/>
-      <c r="H38" s="101"/>
-      <c r="I38" s="101"/>
-      <c r="J38" s="101"/>
-      <c r="K38" s="101"/>
-      <c r="L38" s="101"/>
-      <c r="M38" s="101"/>
-      <c r="N38" s="101"/>
+      <c r="D38" s="102"/>
+      <c r="E38" s="102"/>
+      <c r="F38" s="102"/>
+      <c r="G38" s="102"/>
+      <c r="H38" s="102"/>
+      <c r="I38" s="102"/>
+      <c r="J38" s="102"/>
+      <c r="K38" s="102"/>
+      <c r="L38" s="102"/>
+      <c r="M38" s="102"/>
+      <c r="N38" s="102"/>
     </row>
   </sheetData>
   <mergeCells count="22">

</xml_diff>